<commit_message>
just working on the final table--for >1 and <1 displays
</commit_message>
<xml_diff>
--- a/data/erTimingData-table--FINAL.xlsx
+++ b/data/erTimingData-table--FINAL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\talan\Documents\Krune_git\erFormatAnalysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE70DC7-754B-47D9-90CF-B5AF7146273F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333173CE-8F37-4903-9764-9D1BB8831FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="577" yWindow="1395" windowWidth="22876" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="285" yWindow="1095" windowWidth="22875" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -455,24 +455,6 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -492,6 +474,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -844,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:CU57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M40" workbookViewId="0">
-      <selection activeCell="W43" sqref="W43:AM56"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3782,79 +3782,79 @@
       </c>
     </row>
     <row r="22" spans="3:99" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="Y22" s="1" t="s">
+      <c r="Y22" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="AS22" s="1" t="s">
+      <c r="AS22" s="7" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="23" spans="3:99" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="24" spans="3:99" s="3" customFormat="1" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C24" s="14"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="7" t="s">
+      <c r="C24" s="8"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
-      <c r="S24" s="9"/>
-      <c r="W24" s="14"/>
-      <c r="X24" s="15"/>
-      <c r="Y24" s="7" t="s">
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="20"/>
+      <c r="W24" s="8"/>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="Z24" s="8"/>
-      <c r="AA24" s="8"/>
-      <c r="AB24" s="8"/>
-      <c r="AC24" s="8"/>
-      <c r="AD24" s="8"/>
-      <c r="AE24" s="8"/>
-      <c r="AF24" s="8"/>
-      <c r="AG24" s="8"/>
-      <c r="AH24" s="8"/>
-      <c r="AI24" s="8"/>
-      <c r="AJ24" s="8"/>
-      <c r="AK24" s="8"/>
-      <c r="AL24" s="8"/>
-      <c r="AM24" s="9"/>
-      <c r="AQ24" s="14"/>
-      <c r="AR24" s="15"/>
-      <c r="AS24" s="7" t="s">
+      <c r="Z24" s="19"/>
+      <c r="AA24" s="19"/>
+      <c r="AB24" s="19"/>
+      <c r="AC24" s="19"/>
+      <c r="AD24" s="19"/>
+      <c r="AE24" s="19"/>
+      <c r="AF24" s="19"/>
+      <c r="AG24" s="19"/>
+      <c r="AH24" s="19"/>
+      <c r="AI24" s="19"/>
+      <c r="AJ24" s="19"/>
+      <c r="AK24" s="19"/>
+      <c r="AL24" s="19"/>
+      <c r="AM24" s="20"/>
+      <c r="AQ24" s="8"/>
+      <c r="AR24" s="9"/>
+      <c r="AS24" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="AT24" s="8"/>
-      <c r="AU24" s="8"/>
-      <c r="AV24" s="8"/>
-      <c r="AW24" s="8"/>
-      <c r="AX24" s="8"/>
-      <c r="AY24" s="8"/>
-      <c r="AZ24" s="8"/>
-      <c r="BA24" s="8"/>
-      <c r="BB24" s="8"/>
-      <c r="BC24" s="8"/>
-      <c r="BD24" s="8"/>
-      <c r="BE24" s="8"/>
-      <c r="BF24" s="8"/>
-      <c r="BG24" s="9"/>
+      <c r="AT24" s="19"/>
+      <c r="AU24" s="19"/>
+      <c r="AV24" s="19"/>
+      <c r="AW24" s="19"/>
+      <c r="AX24" s="19"/>
+      <c r="AY24" s="19"/>
+      <c r="AZ24" s="19"/>
+      <c r="BA24" s="19"/>
+      <c r="BB24" s="19"/>
+      <c r="BC24" s="19"/>
+      <c r="BD24" s="19"/>
+      <c r="BE24" s="19"/>
+      <c r="BF24" s="19"/>
+      <c r="BG24" s="20"/>
     </row>
     <row r="25" spans="3:99" s="3" customFormat="1" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C25" s="16"/>
-      <c r="D25" s="17"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="11"/>
       <c r="E25" s="4">
         <v>64</v>
       </c>
@@ -3900,8 +3900,8 @@
       <c r="S25" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="W25" s="16"/>
-      <c r="X25" s="17"/>
+      <c r="W25" s="10"/>
+      <c r="X25" s="11"/>
       <c r="Y25" s="4">
         <v>64</v>
       </c>
@@ -3947,8 +3947,8 @@
       <c r="AM25" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AQ25" s="16"/>
-      <c r="AR25" s="17"/>
+      <c r="AQ25" s="10"/>
+      <c r="AR25" s="11"/>
       <c r="AS25" s="4">
         <v>64</v>
       </c>
@@ -3996,7 +3996,7 @@
       </c>
     </row>
     <row r="26" spans="3:99" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="15" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="5">
@@ -4062,73 +4062,73 @@
         <f t="shared" si="0"/>
         <v>1.0038195519768762</v>
       </c>
-      <c r="W26" s="10" t="s">
+      <c r="W26" s="15" t="s">
         <v>3</v>
       </c>
       <c r="X26" s="5">
         <v>8</v>
       </c>
-      <c r="Y26" s="20">
+      <c r="Y26" s="14">
         <f>IF(Y7="","",IF(AS7=0,"unk",Y7/AS7))</f>
         <v>1.9382477359389898</v>
       </c>
-      <c r="Z26" s="20">
+      <c r="Z26" s="14">
         <f t="shared" ref="Z26:AM26" si="1">IF(Z7="","",IF(AT7=0,"unk",Z7/AT7))</f>
         <v>2.2681338212722815</v>
       </c>
-      <c r="AA26" s="20">
+      <c r="AA26" s="14">
         <f t="shared" si="1"/>
         <v>2.0604847289115842</v>
       </c>
-      <c r="AB26" s="20">
+      <c r="AB26" s="14">
         <f t="shared" si="1"/>
         <v>1.9988138631667929</v>
       </c>
-      <c r="AC26" s="20">
+      <c r="AC26" s="14">
         <f t="shared" si="1"/>
         <v>1.9997353622229572</v>
       </c>
-      <c r="AD26" s="20">
+      <c r="AD26" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE26" s="20">
+      <c r="AE26" s="14">
         <f t="shared" si="1"/>
         <v>1.3891284031107798</v>
       </c>
-      <c r="AF26" s="20">
+      <c r="AF26" s="14">
         <f t="shared" si="1"/>
         <v>1.1449331887465817</v>
       </c>
-      <c r="AG26" s="20">
+      <c r="AG26" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AH26" s="20">
+      <c r="AH26" s="14">
         <f t="shared" si="1"/>
         <v>0.51289328159157321</v>
       </c>
-      <c r="AI26" s="20">
+      <c r="AI26" s="14">
         <f t="shared" si="1"/>
         <v>1.1451012009241317</v>
       </c>
-      <c r="AJ26" s="20">
+      <c r="AJ26" s="14">
         <f t="shared" si="1"/>
         <v>0.16210981965282564</v>
       </c>
-      <c r="AK26" s="20">
+      <c r="AK26" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AL26" s="20">
+      <c r="AL26" s="14">
         <f t="shared" si="1"/>
         <v>3.41786266431943E-2</v>
       </c>
-      <c r="AM26" s="20">
+      <c r="AM26" s="14">
         <f t="shared" si="1"/>
         <v>1.7048906002131867E-2</v>
       </c>
-      <c r="AQ26" s="10" t="s">
+      <c r="AQ26" s="15" t="s">
         <v>3</v>
       </c>
       <c r="AR26" s="5">
@@ -4196,7 +4196,7 @@
       </c>
     </row>
     <row r="27" spans="3:99" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C27" s="11"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="5">
         <v>16</v>
       </c>
@@ -4260,71 +4260,71 @@
         <f t="shared" ref="S27:S37" si="17">IF(S8="","",IF(AM8=0,"unk",S8/AM8))</f>
         <v>4.0039082072351944</v>
       </c>
-      <c r="W27" s="11"/>
+      <c r="W27" s="16"/>
       <c r="X27" s="5">
         <v>16</v>
       </c>
-      <c r="Y27" s="20">
+      <c r="Y27" s="14">
         <f t="shared" ref="Y27:Y29" si="18">IF(Y8="","",IF(AS8=0,"unk",Y8/AS8))</f>
         <v>2.9611927004728478</v>
       </c>
-      <c r="Z27" s="20">
+      <c r="Z27" s="14">
         <f t="shared" ref="Z27:Z29" si="19">IF(Z8="","",IF(AT8=0,"unk",Z8/AT8))</f>
         <v>3.8539384985791081</v>
       </c>
-      <c r="AA27" s="20">
+      <c r="AA27" s="14">
         <f t="shared" ref="AA27:AA29" si="20">IF(AA8="","",IF(AU8=0,"unk",AA8/AU8))</f>
         <v>2.9698066190402455</v>
       </c>
-      <c r="AB27" s="20">
+      <c r="AB27" s="14">
         <f t="shared" ref="AB27:AB29" si="21">IF(AB8="","",IF(AV8=0,"unk",AB8/AV8))</f>
         <v>3.8190410817215019</v>
       </c>
-      <c r="AC27" s="20">
+      <c r="AC27" s="14">
         <f t="shared" ref="AC27:AC29" si="22">IF(AC8="","",IF(AW8=0,"unk",AC8/AW8))</f>
         <v>2.7810101055117933</v>
       </c>
-      <c r="AD27" s="20">
+      <c r="AD27" s="14">
         <f t="shared" ref="AD27:AD29" si="23">IF(AD8="","",IF(AX8=0,"unk",AD8/AX8))</f>
         <v>7.4682901485786468</v>
       </c>
-      <c r="AE27" s="20">
+      <c r="AE27" s="14">
         <f t="shared" ref="AE27:AE29" si="24">IF(AE8="","",IF(AY8=0,"unk",AE8/AY8))</f>
         <v>2.5012144600274273</v>
       </c>
-      <c r="AF27" s="20">
+      <c r="AF27" s="14">
         <f t="shared" ref="AF27:AF29" si="25">IF(AF8="","",IF(AZ8=0,"unk",AF8/AZ8))</f>
         <v>0</v>
       </c>
-      <c r="AG27" s="20">
+      <c r="AG27" s="14">
         <f t="shared" ref="AG27:AG29" si="26">IF(AG8="","",IF(BA8=0,"unk",AG8/BA8))</f>
         <v>1.61582575818715</v>
       </c>
-      <c r="AH27" s="20">
+      <c r="AH27" s="14">
         <f t="shared" ref="AH27:AH29" si="27">IF(AH8="","",IF(BB8=0,"unk",AH8/BB8))</f>
         <v>0</v>
       </c>
-      <c r="AI27" s="20">
+      <c r="AI27" s="14">
         <f t="shared" ref="AI27:AI29" si="28">IF(AI8="","",IF(BC8=0,"unk",AI8/BC8))</f>
         <v>0.30805761409061733</v>
       </c>
-      <c r="AJ27" s="20">
+      <c r="AJ27" s="14">
         <f t="shared" ref="AJ27:AJ29" si="29">IF(AJ8="","",IF(BD8=0,"unk",AJ8/BD8))</f>
         <v>0</v>
       </c>
-      <c r="AK27" s="20">
+      <c r="AK27" s="14">
         <f t="shared" ref="AK27:AK29" si="30">IF(AK8="","",IF(BE8=0,"unk",AK8/BE8))</f>
         <v>0.17048899954883884</v>
       </c>
-      <c r="AL27" s="20">
+      <c r="AL27" s="14">
         <f t="shared" ref="AL27:AL29" si="31">IF(AL8="","",IF(BF8=0,"unk",AL8/BF8))</f>
         <v>0.28076961813688883</v>
       </c>
-      <c r="AM27" s="20">
+      <c r="AM27" s="14">
         <f t="shared" ref="AM27:AM29" si="32">IF(AM8="","",IF(BG8=0,"unk",AM8/BG8))</f>
         <v>1.8123717738797143E-2</v>
       </c>
-      <c r="AQ27" s="11"/>
+      <c r="AQ27" s="16"/>
       <c r="AR27" s="5">
         <v>16</v>
       </c>
@@ -4390,7 +4390,7 @@
       </c>
     </row>
     <row r="28" spans="3:99" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C28" s="11"/>
+      <c r="C28" s="16"/>
       <c r="D28" s="5">
         <v>32</v>
       </c>
@@ -4454,71 +4454,71 @@
         <f t="shared" si="17"/>
         <v>2.9974231962373659</v>
       </c>
-      <c r="W28" s="11"/>
+      <c r="W28" s="16"/>
       <c r="X28" s="5">
         <v>32</v>
       </c>
-      <c r="Y28" s="20">
+      <c r="Y28" s="14">
         <f t="shared" si="18"/>
         <v>5.0231197602164723</v>
       </c>
-      <c r="Z28" s="20">
+      <c r="Z28" s="14">
         <f t="shared" si="19"/>
         <v>5.2521080565328875</v>
       </c>
-      <c r="AA28" s="20">
+      <c r="AA28" s="14">
         <f t="shared" si="20"/>
         <v>4.8957172553438895</v>
       </c>
-      <c r="AB28" s="20">
+      <c r="AB28" s="14">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AC28" s="20">
+      <c r="AC28" s="14">
         <f t="shared" si="22"/>
         <v>4.5997210878906767</v>
       </c>
-      <c r="AD28" s="20">
+      <c r="AD28" s="14">
         <f t="shared" si="23"/>
         <v>31.858611841242684</v>
       </c>
-      <c r="AE28" s="20">
+      <c r="AE28" s="14">
         <f t="shared" si="24"/>
         <v>6.0260176241967134</v>
       </c>
-      <c r="AF28" s="20">
+      <c r="AF28" s="14">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AG28" s="20">
+      <c r="AG28" s="14">
         <f t="shared" si="26"/>
         <v>11.684925102388121</v>
       </c>
-      <c r="AH28" s="20">
+      <c r="AH28" s="14">
         <f t="shared" si="27"/>
         <v>8.4504954538987409</v>
       </c>
-      <c r="AI28" s="20">
+      <c r="AI28" s="14">
         <f t="shared" si="28"/>
         <v>1.1806758842732565</v>
       </c>
-      <c r="AJ28" s="20">
+      <c r="AJ28" s="14">
         <f t="shared" si="29"/>
         <v>2.9454030348418749</v>
       </c>
-      <c r="AK28" s="20">
+      <c r="AK28" s="14">
         <f t="shared" si="30"/>
         <v>0.34129182938566283</v>
       </c>
-      <c r="AL28" s="20">
+      <c r="AL28" s="14">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="AM28" s="20">
+      <c r="AM28" s="14">
         <f t="shared" si="32"/>
         <v>7.5012304067137409E-2</v>
       </c>
-      <c r="AQ28" s="11"/>
+      <c r="AQ28" s="16"/>
       <c r="AR28" s="5">
         <v>32</v>
       </c>
@@ -4584,7 +4584,7 @@
       </c>
     </row>
     <row r="29" spans="3:99" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C29" s="11"/>
+      <c r="C29" s="16"/>
       <c r="D29" s="5">
         <v>64</v>
       </c>
@@ -4648,7 +4648,7 @@
         <f t="shared" si="17"/>
         <v>11.665523456666499</v>
       </c>
-      <c r="W29" s="11"/>
+      <c r="W29" s="16"/>
       <c r="X29" s="5">
         <v>64</v>
       </c>
@@ -4656,63 +4656,63 @@
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="Z29" s="20">
+      <c r="Z29" s="14">
         <f t="shared" si="19"/>
         <v>10.65891592094577</v>
       </c>
-      <c r="AA29" s="20">
+      <c r="AA29" s="14">
         <f t="shared" si="20"/>
         <v>9.1164869261977177</v>
       </c>
-      <c r="AB29" s="20">
+      <c r="AB29" s="14">
         <f t="shared" si="21"/>
         <v>6.9912594835230788</v>
       </c>
-      <c r="AC29" s="20">
+      <c r="AC29" s="14">
         <f t="shared" si="22"/>
         <v>10.992143345432838</v>
       </c>
-      <c r="AD29" s="20">
+      <c r="AD29" s="14">
         <f t="shared" si="23"/>
         <v>7.6925446940929092</v>
       </c>
-      <c r="AE29" s="20">
+      <c r="AE29" s="14">
         <f t="shared" si="24"/>
         <v>5.7302883418513035</v>
       </c>
-      <c r="AF29" s="20">
+      <c r="AF29" s="14">
         <f t="shared" si="25"/>
         <v>4.5450252551975421</v>
       </c>
-      <c r="AG29" s="20">
+      <c r="AG29" s="14">
         <f t="shared" si="26"/>
         <v>6.8963522955039434</v>
       </c>
-      <c r="AH29" s="20">
+      <c r="AH29" s="14">
         <f t="shared" si="27"/>
         <v>2.0682615867731466</v>
       </c>
-      <c r="AI29" s="20">
+      <c r="AI29" s="14">
         <f t="shared" si="28"/>
         <v>2.8133739079122271</v>
       </c>
-      <c r="AJ29" s="20">
+      <c r="AJ29" s="14">
         <f t="shared" si="29"/>
         <v>1.3147390562086445</v>
       </c>
-      <c r="AK29" s="20">
+      <c r="AK29" s="14">
         <f t="shared" si="30"/>
         <v>0.42115408367602725</v>
       </c>
-      <c r="AL29" s="20">
+      <c r="AL29" s="14">
         <f t="shared" si="31"/>
         <v>0.14033478791939863</v>
       </c>
-      <c r="AM29" s="20">
+      <c r="AM29" s="14">
         <f t="shared" si="32"/>
         <v>7.5188911056728328E-2</v>
       </c>
-      <c r="AQ29" s="11"/>
+      <c r="AQ29" s="16"/>
       <c r="AR29" s="5">
         <v>64</v>
       </c>
@@ -4778,7 +4778,7 @@
       </c>
     </row>
     <row r="30" spans="3:99" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C30" s="11"/>
+      <c r="C30" s="16"/>
       <c r="D30" s="5">
         <v>128</v>
       </c>
@@ -4842,7 +4842,7 @@
         <f t="shared" si="17"/>
         <v>20.332137805054632</v>
       </c>
-      <c r="W30" s="11"/>
+      <c r="W30" s="16"/>
       <c r="X30" s="5">
         <v>128</v>
       </c>
@@ -4906,7 +4906,7 @@
         <f t="shared" ref="AM30:AM36" si="62">IF(AM11="","",IF(BG11=0,"unk",INT(AM11/BG11)))</f>
         <v>0</v>
       </c>
-      <c r="AQ30" s="11"/>
+      <c r="AQ30" s="16"/>
       <c r="AR30" s="5">
         <v>128</v>
       </c>
@@ -4972,7 +4972,7 @@
       </c>
     </row>
     <row r="31" spans="3:99" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C31" s="11"/>
+      <c r="C31" s="16"/>
       <c r="D31" s="5">
         <v>256</v>
       </c>
@@ -5036,7 +5036,7 @@
         <f t="shared" si="17"/>
         <v>41.701885368198198</v>
       </c>
-      <c r="W31" s="11"/>
+      <c r="W31" s="16"/>
       <c r="X31" s="5">
         <v>256</v>
       </c>
@@ -5100,7 +5100,7 @@
         <f t="shared" si="62"/>
         <v>0</v>
       </c>
-      <c r="AQ31" s="11"/>
+      <c r="AQ31" s="16"/>
       <c r="AR31" s="5">
         <v>256</v>
       </c>
@@ -5166,7 +5166,7 @@
       </c>
     </row>
     <row r="32" spans="3:99" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C32" s="11"/>
+      <c r="C32" s="16"/>
       <c r="D32" s="5">
         <v>512</v>
       </c>
@@ -5230,7 +5230,7 @@
         <f t="shared" si="17"/>
         <v>74.964923723399409</v>
       </c>
-      <c r="W32" s="11"/>
+      <c r="W32" s="16"/>
       <c r="X32" s="5">
         <v>512</v>
       </c>
@@ -5294,7 +5294,7 @@
         <f t="shared" si="62"/>
         <v>0</v>
       </c>
-      <c r="AQ32" s="11"/>
+      <c r="AQ32" s="16"/>
       <c r="AR32" s="5">
         <v>512</v>
       </c>
@@ -5360,7 +5360,7 @@
       </c>
     </row>
     <row r="33" spans="3:59" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C33" s="11"/>
+      <c r="C33" s="16"/>
       <c r="D33" s="5" t="s">
         <v>48</v>
       </c>
@@ -5424,7 +5424,7 @@
         <f t="shared" si="17"/>
         <v>163.18324069350876</v>
       </c>
-      <c r="W33" s="11"/>
+      <c r="W33" s="16"/>
       <c r="X33" s="5" t="s">
         <v>48</v>
       </c>
@@ -5488,7 +5488,7 @@
         <f t="shared" si="62"/>
         <v>1</v>
       </c>
-      <c r="AQ33" s="11"/>
+      <c r="AQ33" s="16"/>
       <c r="AR33" s="5" t="s">
         <v>48</v>
       </c>
@@ -5554,7 +5554,7 @@
       </c>
     </row>
     <row r="34" spans="3:59" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C34" s="11"/>
+      <c r="C34" s="16"/>
       <c r="D34" s="5" t="s">
         <v>49</v>
       </c>
@@ -5618,7 +5618,7 @@
         <f t="shared" si="17"/>
         <v>313.32274484007388</v>
       </c>
-      <c r="W34" s="11"/>
+      <c r="W34" s="16"/>
       <c r="X34" s="5" t="s">
         <v>49</v>
       </c>
@@ -5682,7 +5682,7 @@
         <f t="shared" si="62"/>
         <v>2</v>
       </c>
-      <c r="AQ34" s="11"/>
+      <c r="AQ34" s="16"/>
       <c r="AR34" s="5" t="s">
         <v>49</v>
       </c>
@@ -5748,7 +5748,7 @@
       </c>
     </row>
     <row r="35" spans="3:59" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C35" s="11"/>
+      <c r="C35" s="16"/>
       <c r="D35" s="5" t="s">
         <v>50</v>
       </c>
@@ -5812,7 +5812,7 @@
         <f t="shared" si="17"/>
         <v>633.2331361518776</v>
       </c>
-      <c r="W35" s="11"/>
+      <c r="W35" s="16"/>
       <c r="X35" s="5" t="s">
         <v>50</v>
       </c>
@@ -5876,7 +5876,7 @@
         <f t="shared" si="62"/>
         <v>5</v>
       </c>
-      <c r="AQ35" s="11"/>
+      <c r="AQ35" s="16"/>
       <c r="AR35" s="5" t="s">
         <v>50</v>
       </c>
@@ -5942,7 +5942,7 @@
       </c>
     </row>
     <row r="36" spans="3:59" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C36" s="11"/>
+      <c r="C36" s="16"/>
       <c r="D36" s="5" t="s">
         <v>51</v>
       </c>
@@ -6006,7 +6006,7 @@
         <f t="shared" si="17"/>
         <v>1242.6000108469548</v>
       </c>
-      <c r="W36" s="11"/>
+      <c r="W36" s="16"/>
       <c r="X36" s="5" t="s">
         <v>51</v>
       </c>
@@ -6070,7 +6070,7 @@
         <f t="shared" si="62"/>
         <v>9</v>
       </c>
-      <c r="AQ36" s="11"/>
+      <c r="AQ36" s="16"/>
       <c r="AR36" s="5" t="s">
         <v>51</v>
       </c>
@@ -6136,7 +6136,7 @@
       </c>
     </row>
     <row r="37" spans="3:59" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C37" s="12"/>
+      <c r="C37" s="17"/>
       <c r="D37" s="5" t="s">
         <v>52</v>
       </c>
@@ -6200,71 +6200,71 @@
         <f t="shared" si="17"/>
         <v>2336.6360687859487</v>
       </c>
-      <c r="W37" s="12"/>
+      <c r="W37" s="17"/>
       <c r="X37" s="5" t="s">
         <v>52</v>
       </c>
       <c r="Y37" s="6" t="str">
-        <f t="shared" ref="Y27:Y37" si="78">IF(Y18="","",IF(AS18=0,"unk",INT(Y18/AS18)))</f>
+        <f t="shared" ref="Y37" si="78">IF(Y18="","",IF(AS18=0,"unk",INT(Y18/AS18)))</f>
         <v/>
       </c>
       <c r="Z37" s="6" t="str">
-        <f t="shared" ref="Z27:Z37" si="79">IF(Z18="","",IF(AT18=0,"unk",INT(Z18/AT18)))</f>
+        <f t="shared" ref="Z37" si="79">IF(Z18="","",IF(AT18=0,"unk",INT(Z18/AT18)))</f>
         <v/>
       </c>
       <c r="AA37" s="6" t="str">
-        <f t="shared" ref="AA27:AA37" si="80">IF(AA18="","",IF(AU18=0,"unk",INT(AA18/AU18)))</f>
+        <f t="shared" ref="AA37" si="80">IF(AA18="","",IF(AU18=0,"unk",INT(AA18/AU18)))</f>
         <v/>
       </c>
       <c r="AB37" s="6" t="str">
-        <f t="shared" ref="AB27:AB37" si="81">IF(AB18="","",IF(AV18=0,"unk",INT(AB18/AV18)))</f>
+        <f t="shared" ref="AB37" si="81">IF(AB18="","",IF(AV18=0,"unk",INT(AB18/AV18)))</f>
         <v/>
       </c>
       <c r="AC37" s="6" t="str">
-        <f t="shared" ref="AC27:AC37" si="82">IF(AC18="","",IF(AW18=0,"unk",INT(AC18/AW18)))</f>
+        <f t="shared" ref="AC37" si="82">IF(AC18="","",IF(AW18=0,"unk",INT(AC18/AW18)))</f>
         <v/>
       </c>
       <c r="AD37" s="6" t="str">
-        <f t="shared" ref="AD27:AD37" si="83">IF(AD18="","",IF(AX18=0,"unk",INT(AD18/AX18)))</f>
+        <f t="shared" ref="AD37" si="83">IF(AD18="","",IF(AX18=0,"unk",INT(AD18/AX18)))</f>
         <v/>
       </c>
       <c r="AE37" s="6" t="str">
-        <f t="shared" ref="AE27:AE37" si="84">IF(AE18="","",IF(AY18=0,"unk",INT(AE18/AY18)))</f>
+        <f t="shared" ref="AE37" si="84">IF(AE18="","",IF(AY18=0,"unk",INT(AE18/AY18)))</f>
         <v/>
       </c>
       <c r="AF37" s="6" t="str">
-        <f t="shared" ref="AF27:AF37" si="85">IF(AF18="","",IF(AZ18=0,"unk",INT(AF18/AZ18)))</f>
+        <f t="shared" ref="AF37" si="85">IF(AF18="","",IF(AZ18=0,"unk",INT(AF18/AZ18)))</f>
         <v/>
       </c>
       <c r="AG37" s="6" t="str">
-        <f t="shared" ref="AG27:AG37" si="86">IF(AG18="","",IF(BA18=0,"unk",INT(AG18/BA18)))</f>
+        <f t="shared" ref="AG37" si="86">IF(AG18="","",IF(BA18=0,"unk",INT(AG18/BA18)))</f>
         <v/>
       </c>
       <c r="AH37" s="6">
-        <f t="shared" ref="AH27:AH37" si="87">IF(AH18="","",IF(BB18=0,"unk",INT(AH18/BB18)))</f>
+        <f t="shared" ref="AH37" si="87">IF(AH18="","",IF(BB18=0,"unk",INT(AH18/BB18)))</f>
         <v>767</v>
       </c>
       <c r="AI37" s="6">
-        <f t="shared" ref="AI27:AI37" si="88">IF(AI18="","",IF(BC18=0,"unk",INT(AI18/BC18)))</f>
+        <f t="shared" ref="AI37" si="88">IF(AI18="","",IF(BC18=0,"unk",INT(AI18/BC18)))</f>
         <v>418</v>
       </c>
       <c r="AJ37" s="6">
-        <f t="shared" ref="AJ27:AJ37" si="89">IF(AJ18="","",IF(BD18=0,"unk",INT(AJ18/BD18)))</f>
+        <f t="shared" ref="AJ37" si="89">IF(AJ18="","",IF(BD18=0,"unk",INT(AJ18/BD18)))</f>
         <v>209</v>
       </c>
       <c r="AK37" s="6">
-        <f t="shared" ref="AK27:AK37" si="90">IF(AK18="","",IF(BE18=0,"unk",INT(AK18/BE18)))</f>
+        <f t="shared" ref="AK37" si="90">IF(AK18="","",IF(BE18=0,"unk",INT(AK18/BE18)))</f>
         <v>73</v>
       </c>
       <c r="AL37" s="6">
-        <f t="shared" ref="AL27:AL37" si="91">IF(AL18="","",IF(BF18=0,"unk",INT(AL18/BF18)))</f>
+        <f t="shared" ref="AL37" si="91">IF(AL18="","",IF(BF18=0,"unk",INT(AL18/BF18)))</f>
         <v>22</v>
       </c>
       <c r="AM37" s="6">
-        <f t="shared" ref="AM27:AM37" si="92">IF(AM18="","",IF(BG18=0,"unk",INT(AM18/BG18)))</f>
+        <f t="shared" ref="AM37" si="92">IF(AM18="","",IF(BG18=0,"unk",INT(AM18/BG18)))</f>
         <v>19</v>
       </c>
-      <c r="AQ37" s="12"/>
+      <c r="AQ37" s="17"/>
       <c r="AR37" s="5" t="s">
         <v>52</v>
       </c>
@@ -6330,58 +6330,58 @@
       </c>
     </row>
     <row r="38" spans="3:59" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="41" spans="3:59" x14ac:dyDescent="0.45">
-      <c r="E41" s="1" t="s">
+    <row r="41" spans="3:59" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="E41" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="Y41" s="1" t="s">
+      <c r="Y41" s="7" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="42" spans="3:59" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="43" spans="3:59" s="3" customFormat="1" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C43" s="14"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="7" t="s">
+      <c r="C43" s="8"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="8"/>
-      <c r="L43" s="8"/>
-      <c r="M43" s="8"/>
-      <c r="N43" s="8"/>
-      <c r="O43" s="8"/>
-      <c r="P43" s="8"/>
-      <c r="Q43" s="8"/>
-      <c r="R43" s="8"/>
-      <c r="S43" s="9"/>
-      <c r="W43" s="14"/>
-      <c r="X43" s="15"/>
-      <c r="Y43" s="7" t="s">
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="19"/>
+      <c r="M43" s="19"/>
+      <c r="N43" s="19"/>
+      <c r="O43" s="19"/>
+      <c r="P43" s="19"/>
+      <c r="Q43" s="19"/>
+      <c r="R43" s="19"/>
+      <c r="S43" s="20"/>
+      <c r="W43" s="8"/>
+      <c r="X43" s="9"/>
+      <c r="Y43" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="Z43" s="8"/>
-      <c r="AA43" s="8"/>
-      <c r="AB43" s="8"/>
-      <c r="AC43" s="8"/>
-      <c r="AD43" s="8"/>
-      <c r="AE43" s="8"/>
-      <c r="AF43" s="8"/>
-      <c r="AG43" s="8"/>
-      <c r="AH43" s="8"/>
-      <c r="AI43" s="8"/>
-      <c r="AJ43" s="8"/>
-      <c r="AK43" s="8"/>
-      <c r="AL43" s="8"/>
-      <c r="AM43" s="9"/>
+      <c r="Z43" s="19"/>
+      <c r="AA43" s="19"/>
+      <c r="AB43" s="19"/>
+      <c r="AC43" s="19"/>
+      <c r="AD43" s="19"/>
+      <c r="AE43" s="19"/>
+      <c r="AF43" s="19"/>
+      <c r="AG43" s="19"/>
+      <c r="AH43" s="19"/>
+      <c r="AI43" s="19"/>
+      <c r="AJ43" s="19"/>
+      <c r="AK43" s="19"/>
+      <c r="AL43" s="19"/>
+      <c r="AM43" s="20"/>
     </row>
     <row r="44" spans="3:59" s="3" customFormat="1" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C44" s="16"/>
-      <c r="D44" s="17"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="11"/>
       <c r="E44" s="4">
         <v>64</v>
       </c>
@@ -6427,8 +6427,8 @@
       <c r="S44" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="W44" s="16"/>
-      <c r="X44" s="17"/>
+      <c r="W44" s="10"/>
+      <c r="X44" s="11"/>
       <c r="Y44" s="4">
         <v>64</v>
       </c>
@@ -6476,1588 +6476,1590 @@
       </c>
     </row>
     <row r="45" spans="3:59" s="3" customFormat="1" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="15" t="s">
         <v>3</v>
       </c>
       <c r="D45" s="5">
         <v>8</v>
       </c>
-      <c r="E45" s="18">
+      <c r="E45" s="12">
         <f>IF(E7="","",IF((Y7+BM7+CG7)=0,"unk",E7/(Y7+BM7+CG7)))</f>
         <v>0.56945511498805934</v>
       </c>
-      <c r="F45" s="18">
+      <c r="F45" s="12">
         <f t="shared" ref="F45:S45" si="94">IF(F7="","",IF((Z7+BN7+CH7)=0,"unk",F7/(Z7+BN7+CH7)))</f>
         <v>0.43862489769338164</v>
       </c>
-      <c r="G45" s="18">
+      <c r="G45" s="12">
         <f t="shared" si="94"/>
         <v>0.49270546281732081</v>
       </c>
-      <c r="H45" s="18">
+      <c r="H45" s="12">
         <f t="shared" si="94"/>
         <v>0.66826170054722656</v>
       </c>
-      <c r="I45" s="18">
+      <c r="I45" s="12">
         <f t="shared" si="94"/>
         <v>0.32150033399775191</v>
       </c>
-      <c r="J45" s="18">
+      <c r="J45" s="12">
         <f t="shared" si="94"/>
         <v>0</v>
       </c>
-      <c r="K45" s="18">
+      <c r="K45" s="12">
         <f t="shared" si="94"/>
         <v>0.93204076037820582</v>
       </c>
-      <c r="L45" s="18">
+      <c r="L45" s="12">
         <f t="shared" si="94"/>
         <v>0.7943067582362896</v>
       </c>
-      <c r="M45" s="18">
+      <c r="M45" s="12">
         <f t="shared" si="94"/>
         <v>2.0070321721877589</v>
       </c>
-      <c r="N45" s="18">
+      <c r="N45" s="12">
         <f t="shared" si="94"/>
         <v>1.3330882844349394</v>
       </c>
-      <c r="O45" s="18">
+      <c r="O45" s="12">
         <f t="shared" si="94"/>
         <v>0.66725677018529816</v>
       </c>
-      <c r="P45" s="18">
+      <c r="P45" s="12">
         <f t="shared" si="94"/>
         <v>1.3156945279615151</v>
       </c>
-      <c r="Q45" s="18">
+      <c r="Q45" s="12">
         <f t="shared" si="94"/>
         <v>0</v>
       </c>
-      <c r="R45" s="18">
+      <c r="R45" s="12">
         <f t="shared" si="94"/>
         <v>0.99969897652016859</v>
       </c>
-      <c r="S45" s="18">
+      <c r="S45" s="12">
         <f t="shared" si="94"/>
         <v>0.65698263630835751</v>
       </c>
-      <c r="W45" s="10" t="s">
+      <c r="W45" s="15" t="s">
         <v>3</v>
       </c>
       <c r="X45" s="5">
         <v>8</v>
       </c>
-      <c r="Y45" s="18">
+      <c r="Y45" s="12">
         <f>IF(Y7="","",IF(AS7=0,"unk",(Y7+BM7+CG7)/AS7))</f>
         <v>5.2230368207816982</v>
       </c>
-      <c r="Z45" s="18">
+      <c r="Z45" s="12">
         <f t="shared" ref="Z45:AM45" si="95">IF(Z7="","",IF(AT7=0,"unk",(Z7+BN7+CH7)/AT7))</f>
         <v>7.4094603622618136</v>
       </c>
-      <c r="AA45" s="18">
+      <c r="AA45" s="12">
         <f t="shared" si="95"/>
         <v>6.7132649245311002</v>
       </c>
-      <c r="AB45" s="18">
+      <c r="AB45" s="12">
         <f t="shared" si="95"/>
         <v>4.4988831828518503</v>
       </c>
-      <c r="AC45" s="18">
+      <c r="AC45" s="12">
         <f t="shared" si="95"/>
         <v>9.3313390135090408</v>
       </c>
-      <c r="AD45" s="18">
+      <c r="AD45" s="12">
         <f t="shared" si="95"/>
         <v>14.695541326833013</v>
       </c>
-      <c r="AE45" s="18">
+      <c r="AE45" s="12">
         <f t="shared" si="95"/>
         <v>2.9803469309420234</v>
       </c>
-      <c r="AF45" s="18">
+      <c r="AF45" s="12">
         <f t="shared" si="95"/>
         <v>2.8313339931418984</v>
       </c>
-      <c r="AG45" s="18">
+      <c r="AG45" s="12">
         <f t="shared" si="95"/>
         <v>1.575540689608391</v>
       </c>
-      <c r="AH45" s="18">
+      <c r="AH45" s="12">
         <f t="shared" si="95"/>
         <v>0.76928850966867579</v>
       </c>
-      <c r="AI45" s="18">
+      <c r="AI45" s="12">
         <f t="shared" si="95"/>
         <v>1.7167343212682784</v>
       </c>
-      <c r="AJ45" s="18">
+      <c r="AJ45" s="12">
         <f t="shared" si="95"/>
         <v>0.24321347942500415</v>
       </c>
-      <c r="AK45" s="18">
+      <c r="AK45" s="12">
         <f t="shared" si="95"/>
         <v>0.16160187142222748</v>
       </c>
-      <c r="AL45" s="18">
+      <c r="AL45" s="12">
         <f t="shared" si="95"/>
         <v>6.8336682340470342E-2</v>
       </c>
-      <c r="AM45" s="18">
+      <c r="AM45" s="12">
         <f t="shared" si="95"/>
         <v>2.6049433027516646E-2</v>
       </c>
     </row>
     <row r="46" spans="3:59" s="3" customFormat="1" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C46" s="11"/>
+      <c r="C46" s="16"/>
       <c r="D46" s="5">
         <v>16</v>
       </c>
-      <c r="E46" s="18">
+      <c r="E46" s="12">
         <f t="shared" ref="E46:E56" si="96">IF(E8="","",IF((Y8+BM8+CG8)=0,"unk",E8/(Y8+BM8+CG8)))</f>
         <v>1.0335892788671073</v>
       </c>
-      <c r="F46" s="18">
+      <c r="F46" s="12">
         <f t="shared" ref="F46:F56" si="97">IF(F8="","",IF((Z8+BN8+CH8)=0,"unk",F8/(Z8+BN8+CH8)))</f>
         <v>0.90215489094945833</v>
       </c>
-      <c r="G46" s="18">
+      <c r="G46" s="12">
         <f t="shared" ref="G46:G56" si="98">IF(G8="","",IF((AA8+BO8+CI8)=0,"unk",G8/(AA8+BO8+CI8)))</f>
         <v>0.88315296998393145</v>
       </c>
-      <c r="H46" s="18">
+      <c r="H46" s="12">
         <f t="shared" ref="H46:H56" si="99">IF(H8="","",IF((AB8+BP8+CJ8)=0,"unk",H8/(AB8+BP8+CJ8)))</f>
         <v>1.38214601982353</v>
       </c>
-      <c r="I46" s="18">
+      <c r="I46" s="12">
         <f t="shared" ref="I46:I56" si="100">IF(I8="","",IF((AC8+BQ8+CK8)=0,"unk",I8/(AC8+BQ8+CK8)))</f>
         <v>1.2620800292813796</v>
       </c>
-      <c r="J46" s="18">
+      <c r="J46" s="12">
         <f t="shared" ref="J46:J56" si="101">IF(J8="","",IF((AD8+BR8+CL8)=0,"unk",J8/(AD8+BR8+CL8)))</f>
         <v>5.2930694474001552</v>
       </c>
-      <c r="K46" s="18">
+      <c r="K46" s="12">
         <f t="shared" ref="K46:K56" si="102">IF(K8="","",IF((AE8+BS8+CM8)=0,"unk",K8/(AE8+BS8+CM8)))</f>
         <v>1.2306962611056269</v>
       </c>
-      <c r="L46" s="18" t="str">
+      <c r="L46" s="12" t="str">
         <f t="shared" ref="L46:L56" si="103">IF(L8="","",IF((AF8+BT8+CN8)=0,"unk",L8/(AF8+BT8+CN8)))</f>
         <v>unk</v>
       </c>
-      <c r="M46" s="18">
+      <c r="M46" s="12">
         <f t="shared" ref="M46:M56" si="104">IF(M8="","",IF((AG8+BU8+CO8)=0,"unk",M8/(AG8+BU8+CO8)))</f>
         <v>1.1312006363997953</v>
       </c>
-      <c r="N46" s="18">
+      <c r="N46" s="12">
         <f t="shared" ref="N46:N56" si="105">IF(N8="","",IF((AH8+BV8+CP8)=0,"unk",N8/(AH8+BV8+CP8)))</f>
         <v>0</v>
       </c>
-      <c r="O46" s="18">
+      <c r="O46" s="12">
         <f t="shared" ref="O46:O56" si="106">IF(O8="","",IF((AI8+BW8+CQ8)=0,"unk",O8/(AI8+BW8+CQ8)))</f>
         <v>1.9758302171813478</v>
       </c>
-      <c r="P46" s="18" t="str">
+      <c r="P46" s="12" t="str">
         <f t="shared" ref="P46:P56" si="107">IF(P8="","",IF((AJ8+BX8+CR8)=0,"unk",P8/(AJ8+BX8+CR8)))</f>
         <v>unk</v>
       </c>
-      <c r="Q46" s="18">
+      <c r="Q46" s="12">
         <f t="shared" ref="Q46:Q56" si="108">IF(Q8="","",IF((AK8+BY8+CS8)=0,"unk",Q8/(AK8+BY8+CS8)))</f>
         <v>0.88901515151515165</v>
       </c>
-      <c r="R46" s="18">
+      <c r="R46" s="12">
         <f t="shared" ref="R46:R56" si="109">IF(R8="","",IF((AL8+BZ8+CT8)=0,"unk",R8/(AL8+BZ8+CT8)))</f>
         <v>2.3019947068331588E-3</v>
       </c>
-      <c r="S46" s="18">
+      <c r="S46" s="12">
         <f t="shared" ref="S46:S56" si="110">IF(S8="","",IF((AM8+CA8+CU8)=0,"unk",S8/(AM8+CA8+CU8)))</f>
         <v>1.609887785321434</v>
       </c>
-      <c r="W46" s="11"/>
+      <c r="W46" s="16"/>
       <c r="X46" s="5">
         <v>16</v>
       </c>
-      <c r="Y46" s="18">
+      <c r="Y46" s="12">
         <f t="shared" ref="Y46:Y56" si="111">IF(Y8="","",IF(AS8=0,"unk",(Y8+BM8+CG8)/AS8))</f>
         <v>7.3329597897289096</v>
       </c>
-      <c r="Z46" s="18">
+      <c r="Z46" s="12">
         <f t="shared" ref="Z46:Z56" si="112">IF(Z8="","",IF(AT8=0,"unk",(Z8+BN8+CH8)/AT8))</f>
         <v>9.2541875321032165</v>
       </c>
-      <c r="AA46" s="18">
+      <c r="AA46" s="12">
         <f t="shared" ref="AA46:AA56" si="113">IF(AA8="","",IF(AU8=0,"unk",(AA8+BO8+CI8)/AU8))</f>
         <v>8.4256091537094768</v>
       </c>
-      <c r="AB46" s="18">
+      <c r="AB46" s="12">
         <f t="shared" ref="AB46:AB56" si="114">IF(AB8="","",IF(AV8=0,"unk",(AB8+BP8+CJ8)/AV8))</f>
         <v>5.7285493986779379</v>
       </c>
-      <c r="AC46" s="18">
+      <c r="AC46" s="12">
         <f t="shared" ref="AC46:AC56" si="115">IF(AC8="","",IF(AW8=0,"unk",(AC8+BQ8+CK8)/AW8))</f>
         <v>5.7227836395440814</v>
       </c>
-      <c r="AD46" s="18">
+      <c r="AD46" s="12">
         <f t="shared" ref="AD46:AD56" si="116">IF(AD8="","",IF(AX8=0,"unk",(AD8+BR8+CL8)/AX8))</f>
         <v>8.7959501240277707</v>
       </c>
-      <c r="AE46" s="18">
+      <c r="AE46" s="12">
         <f t="shared" ref="AE46:AE56" si="117">IF(AE8="","",IF(AY8=0,"unk",(AE8+BS8+CM8)/AY8))</f>
         <v>4.6451842181815053</v>
       </c>
-      <c r="AF46" s="18">
+      <c r="AF46" s="12">
         <f t="shared" ref="AF46:AF56" si="118">IF(AF8="","",IF(AZ8=0,"unk",(AF8+BT8+CN8)/AZ8))</f>
         <v>0</v>
       </c>
-      <c r="AG46" s="18">
+      <c r="AG46" s="12">
         <f t="shared" ref="AG46:AG56" si="119">IF(AG8="","",IF(BA8=0,"unk",(AG8+BU8+CO8)/BA8))</f>
         <v>2.8119170887309064</v>
       </c>
-      <c r="AH46" s="18">
+      <c r="AH46" s="12">
         <f t="shared" ref="AH46:AH56" si="120">IF(AH8="","",IF(BB8=0,"unk",(AH8+BV8+CP8)/BB8))</f>
         <v>8.2212489916750382</v>
       </c>
-      <c r="AI46" s="18">
+      <c r="AI46" s="12">
         <f t="shared" ref="AI46:AI56" si="121">IF(AI8="","",IF(BC8=0,"unk",(AI8+BW8+CQ8)/BC8))</f>
         <v>0.60794030469129201</v>
       </c>
-      <c r="AJ46" s="18">
+      <c r="AJ46" s="12">
         <f t="shared" ref="AJ46:AJ56" si="122">IF(AJ8="","",IF(BD8=0,"unk",(AJ8+BX8+CR8)/BD8))</f>
         <v>0</v>
       </c>
-      <c r="AK46" s="18">
+      <c r="AK46" s="12">
         <f t="shared" ref="AK46:AK56" si="123">IF(AK8="","",IF(BE8=0,"unk",(AK8+BY8+CS8)/BE8))</f>
         <v>0.38363230382310787</v>
       </c>
-      <c r="AL46" s="18">
+      <c r="AL46" s="12">
         <f t="shared" ref="AL46:AL56" si="124">IF(AL8="","",IF(BF8=0,"unk",(AL8+BZ8+CT8)/BF8))</f>
         <v>0.49203289334148992</v>
       </c>
-      <c r="AM46" s="18">
+      <c r="AM46" s="12">
         <f t="shared" ref="AM46:AM56" si="125">IF(AM8="","",IF(BG8=0,"unk",(AM8+CA8+CU8)/BG8))</f>
         <v>4.5075006383438906E-2</v>
       </c>
     </row>
     <row r="47" spans="3:59" s="3" customFormat="1" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C47" s="11"/>
+      <c r="C47" s="16"/>
       <c r="D47" s="5">
         <v>32</v>
       </c>
-      <c r="E47" s="18">
+      <c r="E47" s="12">
         <f t="shared" si="96"/>
         <v>1.4212002659920113</v>
       </c>
-      <c r="F47" s="18">
+      <c r="F47" s="12">
         <f t="shared" si="97"/>
         <v>2.2234372527208208</v>
       </c>
-      <c r="G47" s="18">
+      <c r="G47" s="12">
         <f t="shared" si="98"/>
         <v>1.7728011194854081</v>
       </c>
-      <c r="H47" s="18">
+      <c r="H47" s="12">
         <f t="shared" si="99"/>
         <v>1.3585872640415566</v>
       </c>
-      <c r="I47" s="18">
+      <c r="I47" s="12">
         <f t="shared" si="100"/>
         <v>2.6038440988802267</v>
       </c>
-      <c r="J47" s="18">
+      <c r="J47" s="12">
         <f t="shared" si="101"/>
         <v>0</v>
       </c>
-      <c r="K47" s="18">
+      <c r="K47" s="12">
         <f t="shared" si="102"/>
         <v>2.335748741829724</v>
       </c>
-      <c r="L47" s="18" t="str">
+      <c r="L47" s="12" t="str">
         <f t="shared" si="103"/>
         <v>unk</v>
       </c>
-      <c r="M47" s="18">
+      <c r="M47" s="12">
         <f t="shared" si="104"/>
         <v>0.68134585651262747</v>
       </c>
-      <c r="N47" s="18">
+      <c r="N47" s="12">
         <f t="shared" si="105"/>
         <v>0.99841237324592846</v>
       </c>
-      <c r="O47" s="18">
+      <c r="O47" s="12">
         <f t="shared" si="106"/>
         <v>2.4546795305106617</v>
       </c>
-      <c r="P47" s="18">
+      <c r="P47" s="12">
         <f t="shared" si="107"/>
         <v>0.62465540129155894</v>
       </c>
-      <c r="Q47" s="18">
+      <c r="Q47" s="12">
         <f t="shared" si="108"/>
         <v>1.5482460511236233</v>
       </c>
-      <c r="R47" s="18">
+      <c r="R47" s="12">
         <f t="shared" si="109"/>
         <v>19.805861526357198</v>
       </c>
-      <c r="S47" s="18">
+      <c r="S47" s="12">
         <f t="shared" si="110"/>
         <v>1.4995181537152227</v>
       </c>
-      <c r="W47" s="11"/>
+      <c r="W47" s="16"/>
       <c r="X47" s="5">
         <v>32</v>
       </c>
-      <c r="Y47" s="18">
+      <c r="Y47" s="12">
         <f t="shared" si="111"/>
         <v>14.170801914081341</v>
       </c>
-      <c r="Z47" s="18">
+      <c r="Z47" s="12">
         <f t="shared" si="112"/>
         <v>12.177324229232511</v>
       </c>
-      <c r="AA47" s="18">
+      <c r="AA47" s="12">
         <f t="shared" si="113"/>
         <v>13.672136643155495</v>
       </c>
-      <c r="AB47" s="18">
+      <c r="AB47" s="12">
         <f t="shared" si="114"/>
         <v>16.151650673079082</v>
       </c>
-      <c r="AC47" s="18">
+      <c r="AC47" s="12">
         <f t="shared" si="115"/>
         <v>11.628430518856593</v>
       </c>
-      <c r="AD47" s="18">
+      <c r="AD47" s="12">
         <f t="shared" si="116"/>
         <v>47.79454617726693</v>
       </c>
-      <c r="AE47" s="18">
+      <c r="AE47" s="12">
         <f t="shared" si="117"/>
         <v>9.0293723784969409</v>
       </c>
-      <c r="AF47" s="18">
+      <c r="AF47" s="12">
         <f t="shared" si="118"/>
         <v>0</v>
       </c>
-      <c r="AG47" s="18">
+      <c r="AG47" s="12">
         <f t="shared" si="119"/>
         <v>17.151197800759263</v>
       </c>
-      <c r="AH47" s="18">
+      <c r="AH47" s="12">
         <f t="shared" si="120"/>
         <v>8.4504954538987409</v>
       </c>
-      <c r="AI47" s="18">
+      <c r="AI47" s="12">
         <f t="shared" si="121"/>
         <v>1.9233815015920819</v>
       </c>
-      <c r="AJ47" s="18">
+      <c r="AJ47" s="12">
         <f t="shared" si="122"/>
         <v>4.2768174798805294</v>
       </c>
-      <c r="AK47" s="18">
+      <c r="AK47" s="12">
         <f t="shared" si="123"/>
         <v>0.68142921195253126</v>
       </c>
-      <c r="AL47" s="18">
+      <c r="AL47" s="12">
         <f t="shared" si="124"/>
         <v>3.5308251487674351E-2</v>
       </c>
-      <c r="AM47" s="18">
+      <c r="AM47" s="12">
         <f t="shared" si="125"/>
         <v>0.14994391342110341</v>
       </c>
     </row>
     <row r="48" spans="3:59" s="3" customFormat="1" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C48" s="11"/>
+      <c r="C48" s="16"/>
       <c r="D48" s="5">
         <v>64</v>
       </c>
-      <c r="E48" s="18" t="str">
+      <c r="E48" s="12" t="str">
         <f t="shared" si="96"/>
         <v/>
       </c>
-      <c r="F48" s="18">
+      <c r="F48" s="12">
         <f t="shared" si="97"/>
         <v>3.8371554814980966</v>
       </c>
-      <c r="G48" s="18">
+      <c r="G48" s="12">
         <f t="shared" si="98"/>
         <v>3.4162100111303726</v>
       </c>
-      <c r="H48" s="18">
+      <c r="H48" s="12">
         <f t="shared" si="99"/>
         <v>2.4309689450802034</v>
       </c>
-      <c r="I48" s="18">
+      <c r="I48" s="12">
         <f t="shared" si="100"/>
         <v>4.0334168184172716</v>
       </c>
-      <c r="J48" s="18">
+      <c r="J48" s="12">
         <f t="shared" si="101"/>
         <v>4.37483594945585</v>
       </c>
-      <c r="K48" s="18">
+      <c r="K48" s="12">
         <f t="shared" si="102"/>
         <v>6.5044870148982676</v>
       </c>
-      <c r="L48" s="18">
+      <c r="L48" s="12">
         <f t="shared" si="103"/>
         <v>6.0048073311800501</v>
       </c>
-      <c r="M48" s="18">
+      <c r="M48" s="12">
         <f t="shared" si="104"/>
         <v>4.0000834421558116</v>
       </c>
-      <c r="N48" s="18">
+      <c r="N48" s="12">
         <f t="shared" si="105"/>
         <v>7.9980144660331876</v>
       </c>
-      <c r="O48" s="18">
+      <c r="O48" s="12">
         <f t="shared" si="106"/>
         <v>3.1609272331039757</v>
       </c>
-      <c r="P48" s="18">
+      <c r="P48" s="12">
         <f t="shared" si="107"/>
         <v>3.9995661062205343</v>
       </c>
-      <c r="Q48" s="18">
+      <c r="Q48" s="12">
         <f t="shared" si="108"/>
         <v>5.4417436811045548</v>
       </c>
-      <c r="R48" s="18">
+      <c r="R48" s="12">
         <f t="shared" si="109"/>
         <v>4.8333366657335946</v>
       </c>
-      <c r="S48" s="18">
+      <c r="S48" s="12">
         <f t="shared" si="110"/>
         <v>5.5051094545583421</v>
       </c>
-      <c r="W48" s="11"/>
+      <c r="W48" s="16"/>
       <c r="X48" s="5">
         <v>64</v>
       </c>
-      <c r="Y48" s="18" t="str">
+      <c r="Y48" s="12" t="str">
         <f t="shared" si="111"/>
         <v/>
       </c>
-      <c r="Z48" s="18">
+      <c r="Z48" s="12">
         <f t="shared" si="112"/>
         <v>20.545053671272601</v>
       </c>
-      <c r="AA48" s="18">
+      <c r="AA48" s="12">
         <f t="shared" si="113"/>
         <v>24.781133085746841</v>
       </c>
-      <c r="AB48" s="18">
+      <c r="AB48" s="12">
         <f t="shared" si="114"/>
         <v>35.020772834352968</v>
       </c>
-      <c r="AC48" s="18">
+      <c r="AC48" s="12">
         <f t="shared" si="115"/>
         <v>22.537213198409415</v>
       </c>
-      <c r="AD48" s="18">
+      <c r="AD48" s="12">
         <f t="shared" si="116"/>
         <v>20.321562540919839</v>
       </c>
-      <c r="AE48" s="18">
+      <c r="AE48" s="12">
         <f t="shared" si="117"/>
         <v>11.458208736655584</v>
       </c>
-      <c r="AF48" s="18">
+      <c r="AF48" s="12">
         <f t="shared" si="118"/>
         <v>9.0891402081633625</v>
       </c>
-      <c r="AG48" s="18">
+      <c r="AG48" s="12">
         <f t="shared" si="119"/>
         <v>10.344873722681923</v>
       </c>
-      <c r="AH48" s="18">
+      <c r="AH48" s="12">
         <f t="shared" si="120"/>
         <v>3.1021335821934577</v>
       </c>
-      <c r="AI48" s="18">
+      <c r="AI48" s="12">
         <f t="shared" si="121"/>
         <v>4.6512986666454017</v>
       </c>
-      <c r="AJ48" s="18">
+      <c r="AJ48" s="12">
         <f t="shared" si="122"/>
         <v>1.9718535571517517</v>
       </c>
-      <c r="AK48" s="18">
+      <c r="AK48" s="12">
         <f t="shared" si="123"/>
         <v>0.75768926792756419</v>
       </c>
-      <c r="AL48" s="18">
+      <c r="AL48" s="12">
         <f t="shared" si="124"/>
         <v>0.35136562704316804</v>
       </c>
-      <c r="AM48" s="18">
+      <c r="AM48" s="12">
         <f t="shared" si="125"/>
         <v>0.15932798663743261</v>
       </c>
     </row>
     <row r="49" spans="3:39" s="3" customFormat="1" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C49" s="11"/>
+      <c r="C49" s="16"/>
       <c r="D49" s="5">
         <v>128</v>
       </c>
-      <c r="E49" s="18" t="str">
+      <c r="E49" s="12" t="str">
         <f t="shared" si="96"/>
         <v/>
       </c>
-      <c r="F49" s="18" t="str">
+      <c r="F49" s="12" t="str">
         <f t="shared" si="97"/>
         <v/>
       </c>
-      <c r="G49" s="18">
+      <c r="G49" s="12">
         <f t="shared" si="98"/>
         <v>5.715943441473498</v>
       </c>
-      <c r="H49" s="18">
+      <c r="H49" s="12">
         <f t="shared" si="99"/>
         <v>6.5028129530431036</v>
       </c>
-      <c r="I49" s="18">
+      <c r="I49" s="12">
         <f t="shared" si="100"/>
         <v>7.3813420215910925</v>
       </c>
-      <c r="J49" s="18">
+      <c r="J49" s="12">
         <f t="shared" si="101"/>
         <v>9.0003529862385445</v>
       </c>
-      <c r="K49" s="18">
+      <c r="K49" s="12">
         <f t="shared" si="102"/>
         <v>8.7746604167379481</v>
       </c>
-      <c r="L49" s="18">
+      <c r="L49" s="12">
         <f t="shared" si="103"/>
         <v>6.9370076464706596</v>
       </c>
-      <c r="M49" s="18">
+      <c r="M49" s="12">
         <f t="shared" si="104"/>
         <v>9.0514582555087291</v>
       </c>
-      <c r="N49" s="18">
+      <c r="N49" s="12">
         <f t="shared" si="105"/>
         <v>8.9981267046987234</v>
       </c>
-      <c r="O49" s="18">
+      <c r="O49" s="12">
         <f t="shared" si="106"/>
         <v>7.4297847781061472</v>
       </c>
-      <c r="P49" s="18">
+      <c r="P49" s="12">
         <f t="shared" si="107"/>
         <v>8.6865846625128817</v>
       </c>
-      <c r="Q49" s="18">
+      <c r="Q49" s="12">
         <f t="shared" si="108"/>
         <v>8.7567307049942276</v>
       </c>
-      <c r="R49" s="18">
+      <c r="R49" s="12">
         <f t="shared" si="109"/>
         <v>11.91105378128383</v>
       </c>
-      <c r="S49" s="18">
+      <c r="S49" s="12">
         <f t="shared" si="110"/>
         <v>7.1808711934949629</v>
       </c>
-      <c r="W49" s="11"/>
+      <c r="W49" s="16"/>
       <c r="X49" s="5">
         <v>128</v>
       </c>
-      <c r="Y49" s="18" t="str">
+      <c r="Y49" s="12" t="str">
         <f t="shared" si="111"/>
         <v/>
       </c>
-      <c r="Z49" s="18" t="str">
+      <c r="Z49" s="12" t="str">
         <f t="shared" si="112"/>
         <v/>
       </c>
-      <c r="AA49" s="18">
+      <c r="AA49" s="12">
         <f t="shared" si="113"/>
         <v>45.419967862557861</v>
       </c>
-      <c r="AB49" s="18">
+      <c r="AB49" s="12">
         <f t="shared" si="114"/>
         <v>49.050645068779744</v>
       </c>
-      <c r="AC49" s="18">
+      <c r="AC49" s="12">
         <f t="shared" si="115"/>
         <v>45.729299750151931</v>
       </c>
-      <c r="AD49" s="18">
+      <c r="AD49" s="12">
         <f t="shared" si="116"/>
         <v>38.450483507978888</v>
       </c>
-      <c r="AE49" s="18">
+      <c r="AE49" s="12">
         <f t="shared" si="117"/>
         <v>34.763422699050842</v>
       </c>
-      <c r="AF49" s="18">
+      <c r="AF49" s="12">
         <f t="shared" si="118"/>
         <v>30.93723067313389</v>
       </c>
-      <c r="AG49" s="18">
+      <c r="AG49" s="12">
         <f t="shared" si="119"/>
         <v>16.947779185606493</v>
       </c>
-      <c r="AH49" s="18">
+      <c r="AH49" s="12">
         <f t="shared" si="120"/>
         <v>10.894039140436355</v>
       </c>
-      <c r="AI49" s="18">
+      <c r="AI49" s="12">
         <f t="shared" si="121"/>
         <v>7.2687966524487759</v>
       </c>
-      <c r="AJ49" s="18">
+      <c r="AJ49" s="12">
         <f t="shared" si="122"/>
         <v>3.5542476682254116</v>
       </c>
-      <c r="AK49" s="18">
+      <c r="AK49" s="12">
         <f t="shared" si="123"/>
         <v>1.7583464652883014</v>
       </c>
-      <c r="AL49" s="18">
+      <c r="AL49" s="12">
         <f t="shared" si="124"/>
         <v>0.51627575610238152</v>
       </c>
-      <c r="AM49" s="18">
+      <c r="AM49" s="12">
         <f t="shared" si="125"/>
         <v>0.48365145154321521</v>
       </c>
     </row>
     <row r="50" spans="3:39" s="3" customFormat="1" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C50" s="11"/>
+      <c r="C50" s="16"/>
       <c r="D50" s="5">
         <v>256</v>
       </c>
-      <c r="E50" s="18" t="str">
+      <c r="E50" s="12" t="str">
         <f t="shared" si="96"/>
         <v/>
       </c>
-      <c r="F50" s="18" t="str">
+      <c r="F50" s="12" t="str">
         <f t="shared" si="97"/>
         <v/>
       </c>
-      <c r="G50" s="18" t="str">
+      <c r="G50" s="12" t="str">
         <f t="shared" si="98"/>
         <v/>
       </c>
-      <c r="H50" s="18">
+      <c r="H50" s="12">
         <f t="shared" si="99"/>
         <v>15.829211866713324</v>
       </c>
-      <c r="I50" s="18">
+      <c r="I50" s="12">
         <f t="shared" si="100"/>
         <v>17.811602587988212</v>
       </c>
-      <c r="J50" s="18">
+      <c r="J50" s="12">
         <f t="shared" si="101"/>
         <v>14.629150031120489</v>
       </c>
-      <c r="K50" s="18">
+      <c r="K50" s="12">
         <f t="shared" si="102"/>
         <v>19.386531526209485</v>
       </c>
-      <c r="L50" s="18">
+      <c r="L50" s="12">
         <f t="shared" si="103"/>
         <v>19.433087284242454</v>
       </c>
-      <c r="M50" s="18">
+      <c r="M50" s="12">
         <f t="shared" si="104"/>
         <v>19.805812803765651</v>
       </c>
-      <c r="N50" s="18">
+      <c r="N50" s="12">
         <f t="shared" si="105"/>
         <v>19.329468232499835</v>
       </c>
-      <c r="O50" s="18">
+      <c r="O50" s="12">
         <f t="shared" si="106"/>
         <v>20.648215433799113</v>
       </c>
-      <c r="P50" s="18">
+      <c r="P50" s="12">
         <f t="shared" si="107"/>
         <v>18.258132474130981</v>
       </c>
-      <c r="Q50" s="18">
+      <c r="Q50" s="12">
         <f t="shared" si="108"/>
         <v>14.371458711440654</v>
       </c>
-      <c r="R50" s="18">
+      <c r="R50" s="12">
         <f t="shared" si="109"/>
         <v>23.021041861571149</v>
       </c>
-      <c r="S50" s="18">
+      <c r="S50" s="12">
         <f t="shared" si="110"/>
         <v>20.565089049940088</v>
       </c>
-      <c r="W50" s="11"/>
+      <c r="W50" s="16"/>
       <c r="X50" s="5">
         <v>256</v>
       </c>
-      <c r="Y50" s="18" t="str">
+      <c r="Y50" s="12" t="str">
         <f t="shared" si="111"/>
         <v/>
       </c>
-      <c r="Z50" s="18" t="str">
+      <c r="Z50" s="12" t="str">
         <f t="shared" si="112"/>
         <v/>
       </c>
-      <c r="AA50" s="18" t="str">
+      <c r="AA50" s="12" t="str">
         <f t="shared" si="113"/>
         <v/>
       </c>
-      <c r="AB50" s="18">
+      <c r="AB50" s="12">
         <f t="shared" si="114"/>
         <v>75.116879215422841</v>
       </c>
-      <c r="AC50" s="18">
+      <c r="AC50" s="12">
         <f t="shared" si="115"/>
         <v>69.722993425492106</v>
       </c>
-      <c r="AD50" s="18">
+      <c r="AD50" s="12">
         <f t="shared" si="116"/>
         <v>75.825035971223016</v>
       </c>
-      <c r="AE50" s="18">
+      <c r="AE50" s="12">
         <f t="shared" si="117"/>
         <v>58.427745626737099</v>
       </c>
-      <c r="AF50" s="18">
+      <c r="AF50" s="12">
         <f t="shared" si="118"/>
         <v>42.821315641521167</v>
       </c>
-      <c r="AG50" s="18">
+      <c r="AG50" s="12">
         <f t="shared" si="119"/>
         <v>30.257840778368173</v>
       </c>
-      <c r="AH50" s="18">
+      <c r="AH50" s="12">
         <f t="shared" si="120"/>
         <v>18.801012180902529</v>
       </c>
-      <c r="AI50" s="18">
+      <c r="AI50" s="12">
         <f t="shared" si="121"/>
         <v>10.364490629213476</v>
       </c>
-      <c r="AJ50" s="18">
+      <c r="AJ50" s="12">
         <f t="shared" si="122"/>
         <v>6.4621957477932481</v>
       </c>
-      <c r="AK50" s="18">
+      <c r="AK50" s="12">
         <f t="shared" si="123"/>
         <v>4.1609852214256229</v>
       </c>
-      <c r="AL50" s="18">
+      <c r="AL50" s="12">
         <f t="shared" si="124"/>
         <v>1.0782377089720026</v>
       </c>
-      <c r="AM50" s="18">
+      <c r="AM50" s="12">
         <f t="shared" si="125"/>
         <v>0.63011373445521579</v>
       </c>
     </row>
     <row r="51" spans="3:39" s="3" customFormat="1" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C51" s="11"/>
+      <c r="C51" s="16"/>
       <c r="D51" s="5">
         <v>512</v>
       </c>
-      <c r="E51" s="18" t="str">
+      <c r="E51" s="12" t="str">
         <f t="shared" si="96"/>
         <v/>
       </c>
-      <c r="F51" s="18" t="str">
+      <c r="F51" s="12" t="str">
         <f t="shared" si="97"/>
         <v/>
       </c>
-      <c r="G51" s="18" t="str">
+      <c r="G51" s="12" t="str">
         <f t="shared" si="98"/>
         <v/>
       </c>
-      <c r="H51" s="18" t="str">
+      <c r="H51" s="12" t="str">
         <f t="shared" si="99"/>
         <v/>
       </c>
-      <c r="I51" s="18">
+      <c r="I51" s="12">
         <f t="shared" si="100"/>
         <v>27.182181555962003</v>
       </c>
-      <c r="J51" s="18">
+      <c r="J51" s="12">
         <f t="shared" si="101"/>
         <v>23.325308324851928</v>
       </c>
-      <c r="K51" s="18">
+      <c r="K51" s="12">
         <f t="shared" si="102"/>
         <v>31.052016934653526</v>
       </c>
-      <c r="L51" s="18">
+      <c r="L51" s="12">
         <f t="shared" si="103"/>
         <v>28.352445622571626</v>
       </c>
-      <c r="M51" s="18">
+      <c r="M51" s="12">
         <f t="shared" si="104"/>
         <v>31.714939404446188</v>
       </c>
-      <c r="N51" s="18">
+      <c r="N51" s="12">
         <f t="shared" si="105"/>
         <v>24.755225149836033</v>
       </c>
-      <c r="O51" s="18">
+      <c r="O51" s="12">
         <f t="shared" si="106"/>
         <v>32.391316679522937</v>
       </c>
-      <c r="P51" s="18">
+      <c r="P51" s="12">
         <f t="shared" si="107"/>
         <v>34.030401036856951</v>
       </c>
-      <c r="Q51" s="18">
+      <c r="Q51" s="12">
         <f t="shared" si="108"/>
         <v>33.567570993839709</v>
       </c>
-      <c r="R51" s="18">
+      <c r="R51" s="12">
         <f t="shared" si="109"/>
         <v>35.841741889027851</v>
       </c>
-      <c r="S51" s="18">
+      <c r="S51" s="12">
         <f t="shared" si="110"/>
         <v>24.955165456102687</v>
       </c>
-      <c r="W51" s="11"/>
+      <c r="W51" s="16"/>
       <c r="X51" s="5">
         <v>512</v>
       </c>
-      <c r="Y51" s="18" t="str">
+      <c r="Y51" s="12" t="str">
         <f t="shared" si="111"/>
         <v/>
       </c>
-      <c r="Z51" s="18" t="str">
+      <c r="Z51" s="12" t="str">
         <f t="shared" si="112"/>
         <v/>
       </c>
-      <c r="AA51" s="18" t="str">
+      <c r="AA51" s="12" t="str">
         <f t="shared" si="113"/>
         <v/>
       </c>
-      <c r="AB51" s="18" t="str">
+      <c r="AB51" s="12" t="str">
         <f t="shared" si="114"/>
         <v/>
       </c>
-      <c r="AC51" s="18">
+      <c r="AC51" s="12">
         <f t="shared" si="115"/>
         <v>110.50286744072832</v>
       </c>
-      <c r="AD51" s="18">
+      <c r="AD51" s="12">
         <f t="shared" si="116"/>
         <v>197.53421679527648</v>
       </c>
-      <c r="AE51" s="18">
+      <c r="AE51" s="12">
         <f t="shared" si="117"/>
         <v>150.23129099454266</v>
       </c>
-      <c r="AF51" s="18">
+      <c r="AF51" s="12">
         <f t="shared" si="118"/>
         <v>108.0734711984712</v>
       </c>
-      <c r="AG51" s="18">
+      <c r="AG51" s="12">
         <f t="shared" si="119"/>
         <v>66.967793439407188</v>
       </c>
-      <c r="AH51" s="18">
+      <c r="AH51" s="12">
         <f t="shared" si="120"/>
         <v>57.762622338137938</v>
       </c>
-      <c r="AI51" s="18">
+      <c r="AI51" s="12">
         <f t="shared" si="121"/>
         <v>25.986613956382946</v>
       </c>
-      <c r="AJ51" s="18">
+      <c r="AJ51" s="12">
         <f t="shared" si="122"/>
         <v>14.269309301175365</v>
       </c>
-      <c r="AK51" s="18">
+      <c r="AK51" s="12">
         <f t="shared" si="123"/>
         <v>6.8849034758042231</v>
       </c>
-      <c r="AL51" s="18">
+      <c r="AL51" s="12">
         <f t="shared" si="124"/>
         <v>2.8535813368787788</v>
       </c>
-      <c r="AM51" s="18">
+      <c r="AM51" s="12">
         <f t="shared" si="125"/>
         <v>1.853398780797038</v>
       </c>
     </row>
     <row r="52" spans="3:39" s="3" customFormat="1" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C52" s="11"/>
+      <c r="C52" s="16"/>
       <c r="D52" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E52" s="18" t="str">
+      <c r="E52" s="12" t="str">
         <f t="shared" si="96"/>
         <v/>
       </c>
-      <c r="F52" s="18" t="str">
+      <c r="F52" s="12" t="str">
         <f t="shared" si="97"/>
         <v/>
       </c>
-      <c r="G52" s="18" t="str">
+      <c r="G52" s="12" t="str">
         <f t="shared" si="98"/>
         <v/>
       </c>
-      <c r="H52" s="18" t="str">
+      <c r="H52" s="12" t="str">
         <f t="shared" si="99"/>
         <v/>
       </c>
-      <c r="I52" s="18" t="str">
+      <c r="I52" s="12" t="str">
         <f t="shared" si="100"/>
         <v/>
       </c>
-      <c r="J52" s="18">
+      <c r="J52" s="12">
         <f t="shared" si="101"/>
         <v>58.383650210511881</v>
       </c>
-      <c r="K52" s="18">
+      <c r="K52" s="12">
         <f t="shared" si="102"/>
         <v>65.448161971732816</v>
       </c>
-      <c r="L52" s="18">
+      <c r="L52" s="12">
         <f t="shared" si="103"/>
         <v>67.615900389635669</v>
       </c>
-      <c r="M52" s="18">
+      <c r="M52" s="12">
         <f t="shared" si="104"/>
         <v>65.745869452197738</v>
       </c>
-      <c r="N52" s="18">
+      <c r="N52" s="12">
         <f t="shared" si="105"/>
         <v>61.014996638569691</v>
       </c>
-      <c r="O52" s="18">
+      <c r="O52" s="12">
         <f t="shared" si="106"/>
         <v>71.28355612276755</v>
       </c>
-      <c r="P52" s="18">
+      <c r="P52" s="12">
         <f t="shared" si="107"/>
         <v>66.44795274644261</v>
       </c>
-      <c r="Q52" s="18">
+      <c r="Q52" s="12">
         <f t="shared" si="108"/>
         <v>75.1785535643385</v>
       </c>
-      <c r="R52" s="18">
+      <c r="R52" s="12">
         <f t="shared" si="109"/>
         <v>61.736213523504304</v>
       </c>
-      <c r="S52" s="18">
+      <c r="S52" s="12">
         <f t="shared" si="110"/>
         <v>62.258459236085734</v>
       </c>
-      <c r="W52" s="11"/>
+      <c r="W52" s="16"/>
       <c r="X52" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="Y52" s="18" t="str">
+      <c r="Y52" s="12" t="str">
         <f t="shared" si="111"/>
         <v/>
       </c>
-      <c r="Z52" s="18" t="str">
+      <c r="Z52" s="12" t="str">
         <f t="shared" si="112"/>
         <v/>
       </c>
-      <c r="AA52" s="18" t="str">
+      <c r="AA52" s="12" t="str">
         <f t="shared" si="113"/>
         <v/>
       </c>
-      <c r="AB52" s="18" t="str">
+      <c r="AB52" s="12" t="str">
         <f t="shared" si="114"/>
         <v/>
       </c>
-      <c r="AC52" s="18" t="str">
+      <c r="AC52" s="12" t="str">
         <f t="shared" si="115"/>
         <v/>
       </c>
-      <c r="AD52" s="18">
+      <c r="AD52" s="12">
         <f t="shared" si="116"/>
         <v>248.03382045654661</v>
       </c>
-      <c r="AE52" s="18">
+      <c r="AE52" s="12">
         <f t="shared" si="117"/>
         <v>216.6095527276353</v>
       </c>
-      <c r="AF52" s="18">
+      <c r="AF52" s="12">
         <f t="shared" si="118"/>
         <v>209.08912334703629</v>
       </c>
-      <c r="AG52" s="18">
+      <c r="AG52" s="12">
         <f t="shared" si="119"/>
         <v>136.02138538581715</v>
       </c>
-      <c r="AH52" s="18">
+      <c r="AH52" s="12">
         <f t="shared" si="120"/>
         <v>91.040131701873023</v>
       </c>
-      <c r="AI52" s="18">
+      <c r="AI52" s="12">
         <f t="shared" si="121"/>
         <v>41.096553121332363</v>
       </c>
-      <c r="AJ52" s="18">
+      <c r="AJ52" s="12">
         <f t="shared" si="122"/>
         <v>28.137665035560097</v>
       </c>
-      <c r="AK52" s="18">
+      <c r="AK52" s="12">
         <f t="shared" si="123"/>
         <v>11.426048111449862</v>
       </c>
-      <c r="AL52" s="18">
+      <c r="AL52" s="12">
         <f t="shared" si="124"/>
         <v>5.960996483834891</v>
       </c>
-      <c r="AM52" s="18">
+      <c r="AM52" s="12">
         <f t="shared" si="125"/>
         <v>3.022501850693823</v>
       </c>
     </row>
     <row r="53" spans="3:39" s="3" customFormat="1" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C53" s="11"/>
+      <c r="C53" s="16"/>
       <c r="D53" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E53" s="18" t="str">
+      <c r="E53" s="12" t="str">
         <f t="shared" si="96"/>
         <v/>
       </c>
-      <c r="F53" s="18" t="str">
+      <c r="F53" s="12" t="str">
         <f t="shared" si="97"/>
         <v/>
       </c>
-      <c r="G53" s="18" t="str">
+      <c r="G53" s="12" t="str">
         <f t="shared" si="98"/>
         <v/>
       </c>
-      <c r="H53" s="18" t="str">
+      <c r="H53" s="12" t="str">
         <f t="shared" si="99"/>
         <v/>
       </c>
-      <c r="I53" s="18" t="str">
+      <c r="I53" s="12" t="str">
         <f t="shared" si="100"/>
         <v/>
       </c>
-      <c r="J53" s="18" t="str">
+      <c r="J53" s="12" t="str">
         <f t="shared" si="101"/>
         <v/>
       </c>
-      <c r="K53" s="18">
+      <c r="K53" s="12">
         <f t="shared" si="102"/>
         <v>101.86001451702975</v>
       </c>
-      <c r="L53" s="18">
+      <c r="L53" s="12">
         <f t="shared" si="103"/>
         <v>114.76064926268624</v>
       </c>
-      <c r="M53" s="18">
+      <c r="M53" s="12">
         <f t="shared" si="104"/>
         <v>103.68756217615335</v>
       </c>
-      <c r="N53" s="18">
+      <c r="N53" s="12">
         <f t="shared" si="105"/>
         <v>130.11912513617344</v>
       </c>
-      <c r="O53" s="18">
+      <c r="O53" s="12">
         <f t="shared" si="106"/>
         <v>127.28478032020749</v>
       </c>
-      <c r="P53" s="18">
+      <c r="P53" s="12">
         <f t="shared" si="107"/>
         <v>132.29025467113362</v>
       </c>
-      <c r="Q53" s="18">
+      <c r="Q53" s="12">
         <f t="shared" si="108"/>
         <v>125.85314221311678</v>
       </c>
-      <c r="R53" s="18">
+      <c r="R53" s="12">
         <f t="shared" si="109"/>
         <v>133.77313321743327</v>
       </c>
-      <c r="S53" s="18">
+      <c r="S53" s="12">
         <f t="shared" si="110"/>
         <v>126.28806393130853</v>
       </c>
-      <c r="W53" s="11"/>
+      <c r="W53" s="16"/>
       <c r="X53" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="Y53" s="18" t="str">
+      <c r="Y53" s="12" t="str">
         <f t="shared" si="111"/>
         <v/>
       </c>
-      <c r="Z53" s="18" t="str">
+      <c r="Z53" s="12" t="str">
         <f t="shared" si="112"/>
         <v/>
       </c>
-      <c r="AA53" s="18" t="str">
+      <c r="AA53" s="12" t="str">
         <f t="shared" si="113"/>
         <v/>
       </c>
-      <c r="AB53" s="18" t="str">
+      <c r="AB53" s="12" t="str">
         <f t="shared" si="114"/>
         <v/>
       </c>
-      <c r="AC53" s="18" t="str">
+      <c r="AC53" s="12" t="str">
         <f t="shared" si="115"/>
         <v/>
       </c>
-      <c r="AD53" s="18" t="str">
+      <c r="AD53" s="12" t="str">
         <f t="shared" si="116"/>
         <v/>
       </c>
-      <c r="AE53" s="18">
+      <c r="AE53" s="12">
         <f t="shared" si="117"/>
         <v>526.62186931839267</v>
       </c>
-      <c r="AF53" s="18">
+      <c r="AF53" s="12">
         <f t="shared" si="118"/>
         <v>515.21632987562077</v>
       </c>
-      <c r="AG53" s="18">
+      <c r="AG53" s="12">
         <f t="shared" si="119"/>
         <v>371.67526720749413</v>
       </c>
-      <c r="AH53" s="18">
+      <c r="AH53" s="12">
         <f t="shared" si="120"/>
         <v>184.3580115084101</v>
       </c>
-      <c r="AI53" s="18">
+      <c r="AI53" s="12">
         <f t="shared" si="121"/>
         <v>103.57582712494832</v>
       </c>
-      <c r="AJ53" s="18">
+      <c r="AJ53" s="12">
         <f t="shared" si="122"/>
         <v>54.672932327156509</v>
       </c>
-      <c r="AK53" s="18">
+      <c r="AK53" s="12">
         <f t="shared" si="123"/>
         <v>26.619974376814721</v>
       </c>
-      <c r="AL53" s="18">
+      <c r="AL53" s="12">
         <f t="shared" si="124"/>
         <v>8.5979462752602664</v>
       </c>
-      <c r="AM53" s="18">
+      <c r="AM53" s="12">
         <f t="shared" si="125"/>
         <v>7.4375160430809437</v>
       </c>
     </row>
     <row r="54" spans="3:39" s="3" customFormat="1" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C54" s="11"/>
+      <c r="C54" s="16"/>
       <c r="D54" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E54" s="18" t="str">
+      <c r="E54" s="12" t="str">
         <f t="shared" si="96"/>
         <v/>
       </c>
-      <c r="F54" s="18" t="str">
+      <c r="F54" s="12" t="str">
         <f t="shared" si="97"/>
         <v/>
       </c>
-      <c r="G54" s="18" t="str">
+      <c r="G54" s="12" t="str">
         <f t="shared" si="98"/>
         <v/>
       </c>
-      <c r="H54" s="18" t="str">
+      <c r="H54" s="12" t="str">
         <f t="shared" si="99"/>
         <v/>
       </c>
-      <c r="I54" s="18" t="str">
+      <c r="I54" s="12" t="str">
         <f t="shared" si="100"/>
         <v/>
       </c>
-      <c r="J54" s="18" t="str">
+      <c r="J54" s="12" t="str">
         <f t="shared" si="101"/>
         <v/>
       </c>
-      <c r="K54" s="18" t="str">
+      <c r="K54" s="12" t="str">
         <f t="shared" si="102"/>
         <v/>
       </c>
-      <c r="L54" s="18">
+      <c r="L54" s="12">
         <f t="shared" si="103"/>
         <v>190.74961574408493</v>
       </c>
-      <c r="M54" s="18">
+      <c r="M54" s="12">
         <f t="shared" si="104"/>
         <v>279.67309141384959</v>
       </c>
-      <c r="N54" s="18">
+      <c r="N54" s="12">
         <f t="shared" si="105"/>
         <v>262.78721296607074</v>
       </c>
-      <c r="O54" s="18">
+      <c r="O54" s="12">
         <f t="shared" si="106"/>
         <v>211.09480073111757</v>
       </c>
-      <c r="P54" s="18">
+      <c r="P54" s="12">
         <f t="shared" si="107"/>
         <v>277.27695166972484</v>
       </c>
-      <c r="Q54" s="18">
+      <c r="Q54" s="12">
         <f t="shared" si="108"/>
         <v>301.28106694235936</v>
       </c>
-      <c r="R54" s="18">
+      <c r="R54" s="12">
         <f t="shared" si="109"/>
         <v>276.45780489036184</v>
       </c>
-      <c r="S54" s="18">
+      <c r="S54" s="12">
         <f t="shared" si="110"/>
         <v>297.94730767274928</v>
       </c>
-      <c r="W54" s="11"/>
+      <c r="W54" s="16"/>
       <c r="X54" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="Y54" s="18" t="str">
+      <c r="Y54" s="12" t="str">
         <f t="shared" si="111"/>
         <v/>
       </c>
-      <c r="Z54" s="18" t="str">
+      <c r="Z54" s="12" t="str">
         <f t="shared" si="112"/>
         <v/>
       </c>
-      <c r="AA54" s="18" t="str">
+      <c r="AA54" s="12" t="str">
         <f t="shared" si="113"/>
         <v/>
       </c>
-      <c r="AB54" s="18" t="str">
+      <c r="AB54" s="12" t="str">
         <f t="shared" si="114"/>
         <v/>
       </c>
-      <c r="AC54" s="18" t="str">
+      <c r="AC54" s="12" t="str">
         <f t="shared" si="115"/>
         <v/>
       </c>
-      <c r="AD54" s="18" t="str">
+      <c r="AD54" s="12" t="str">
         <f t="shared" si="116"/>
         <v/>
       </c>
-      <c r="AE54" s="18" t="str">
+      <c r="AE54" s="12" t="str">
         <f t="shared" si="117"/>
         <v/>
       </c>
-      <c r="AF54" s="18">
+      <c r="AF54" s="12">
         <f t="shared" si="118"/>
         <v>860.60848094560845</v>
       </c>
-      <c r="AG54" s="18">
+      <c r="AG54" s="12">
         <f t="shared" si="119"/>
         <v>611.97964892837365</v>
       </c>
-      <c r="AH54" s="18">
+      <c r="AH54" s="12">
         <f t="shared" si="120"/>
         <v>360.39303863739195</v>
       </c>
-      <c r="AI54" s="18">
+      <c r="AI54" s="12">
         <f t="shared" si="121"/>
         <v>264.23205187242826</v>
       </c>
-      <c r="AJ54" s="18">
+      <c r="AJ54" s="12">
         <f t="shared" si="122"/>
         <v>108.62887002142428</v>
       </c>
-      <c r="AK54" s="18">
+      <c r="AK54" s="12">
         <f t="shared" si="123"/>
         <v>44.20057329706318</v>
       </c>
-      <c r="AL54" s="18">
+      <c r="AL54" s="12">
         <f t="shared" si="124"/>
         <v>15.374659479892761</v>
       </c>
-      <c r="AM54" s="18">
+      <c r="AM54" s="12">
         <f t="shared" si="125"/>
         <v>11.908308983304414</v>
       </c>
     </row>
     <row r="55" spans="3:39" s="3" customFormat="1" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C55" s="11"/>
+      <c r="C55" s="16"/>
       <c r="D55" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E55" s="18" t="str">
+      <c r="E55" s="12" t="str">
         <f t="shared" si="96"/>
         <v/>
       </c>
-      <c r="F55" s="18" t="str">
+      <c r="F55" s="12" t="str">
         <f t="shared" si="97"/>
         <v/>
       </c>
-      <c r="G55" s="18" t="str">
+      <c r="G55" s="12" t="str">
         <f t="shared" si="98"/>
         <v/>
       </c>
-      <c r="H55" s="18" t="str">
+      <c r="H55" s="12" t="str">
         <f t="shared" si="99"/>
         <v/>
       </c>
-      <c r="I55" s="18" t="str">
+      <c r="I55" s="12" t="str">
         <f t="shared" si="100"/>
         <v/>
       </c>
-      <c r="J55" s="18" t="str">
+      <c r="J55" s="12" t="str">
         <f t="shared" si="101"/>
         <v/>
       </c>
-      <c r="K55" s="18" t="str">
+      <c r="K55" s="12" t="str">
         <f t="shared" si="102"/>
         <v/>
       </c>
-      <c r="L55" s="18" t="str">
+      <c r="L55" s="12" t="str">
         <f t="shared" si="103"/>
         <v/>
       </c>
-      <c r="M55" s="18">
+      <c r="M55" s="12">
         <f t="shared" si="104"/>
         <v>431.35066480380794</v>
       </c>
-      <c r="N55" s="18">
+      <c r="N55" s="12">
         <f t="shared" si="105"/>
         <v>469.18742553181409</v>
       </c>
-      <c r="O55" s="18">
+      <c r="O55" s="12">
         <f t="shared" si="106"/>
         <v>474.61086920754838</v>
       </c>
-      <c r="P55" s="18">
+      <c r="P55" s="12">
         <f t="shared" si="107"/>
         <v>371.3429219132932</v>
       </c>
-      <c r="Q55" s="18">
+      <c r="Q55" s="12">
         <f t="shared" si="108"/>
         <v>470.93494973764621</v>
       </c>
-      <c r="R55" s="18">
+      <c r="R55" s="12">
         <f t="shared" si="109"/>
         <v>463.31648115808122</v>
       </c>
-      <c r="S55" s="18">
+      <c r="S55" s="12">
         <f t="shared" si="110"/>
         <v>483.72022018436144</v>
       </c>
-      <c r="W55" s="11"/>
+      <c r="W55" s="16"/>
       <c r="X55" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="Y55" s="18" t="str">
+      <c r="Y55" s="12" t="str">
         <f t="shared" si="111"/>
         <v/>
       </c>
-      <c r="Z55" s="18" t="str">
+      <c r="Z55" s="12" t="str">
         <f t="shared" si="112"/>
         <v/>
       </c>
-      <c r="AA55" s="18" t="str">
+      <c r="AA55" s="12" t="str">
         <f t="shared" si="113"/>
         <v/>
       </c>
-      <c r="AB55" s="18" t="str">
+      <c r="AB55" s="12" t="str">
         <f t="shared" si="114"/>
         <v/>
       </c>
-      <c r="AC55" s="18" t="str">
+      <c r="AC55" s="12" t="str">
         <f t="shared" si="115"/>
         <v/>
       </c>
-      <c r="AD55" s="18" t="str">
+      <c r="AD55" s="12" t="str">
         <f t="shared" si="116"/>
         <v/>
       </c>
-      <c r="AE55" s="18" t="str">
+      <c r="AE55" s="12" t="str">
         <f t="shared" si="117"/>
         <v/>
       </c>
-      <c r="AF55" s="18" t="str">
+      <c r="AF55" s="12" t="str">
         <f t="shared" si="118"/>
         <v/>
       </c>
-      <c r="AG55" s="18">
+      <c r="AG55" s="12">
         <f t="shared" si="119"/>
         <v>1257.7431198495187</v>
       </c>
-      <c r="AH55" s="18">
+      <c r="AH55" s="12">
         <f t="shared" si="120"/>
         <v>904.55043177463097</v>
       </c>
-      <c r="AI55" s="18">
+      <c r="AI55" s="12">
         <f t="shared" si="121"/>
         <v>550.67492548543157</v>
       </c>
-      <c r="AJ55" s="18">
+      <c r="AJ55" s="12">
         <f t="shared" si="122"/>
         <v>315.09366733833463</v>
       </c>
-      <c r="AK55" s="18">
+      <c r="AK55" s="12">
         <f t="shared" si="123"/>
         <v>98.006952619545743</v>
       </c>
-      <c r="AL55" s="18">
+      <c r="AL55" s="12">
         <f t="shared" si="124"/>
         <v>28.257958091547692</v>
       </c>
-      <c r="AM55" s="18">
+      <c r="AM55" s="12">
         <f t="shared" si="125"/>
         <v>25.54433715581532</v>
       </c>
     </row>
     <row r="56" spans="3:39" s="3" customFormat="1" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C56" s="12"/>
+      <c r="C56" s="17"/>
       <c r="D56" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E56" s="18" t="str">
+      <c r="E56" s="12" t="str">
         <f t="shared" si="96"/>
         <v/>
       </c>
-      <c r="F56" s="18" t="str">
+      <c r="F56" s="12" t="str">
         <f t="shared" si="97"/>
         <v/>
       </c>
-      <c r="G56" s="18" t="str">
+      <c r="G56" s="12" t="str">
         <f t="shared" si="98"/>
         <v/>
       </c>
-      <c r="H56" s="18" t="str">
+      <c r="H56" s="12" t="str">
         <f t="shared" si="99"/>
         <v/>
       </c>
-      <c r="I56" s="18" t="str">
+      <c r="I56" s="12" t="str">
         <f t="shared" si="100"/>
         <v/>
       </c>
-      <c r="J56" s="18" t="str">
+      <c r="J56" s="12" t="str">
         <f t="shared" si="101"/>
         <v/>
       </c>
-      <c r="K56" s="18" t="str">
+      <c r="K56" s="12" t="str">
         <f t="shared" si="102"/>
         <v/>
       </c>
-      <c r="L56" s="18" t="str">
+      <c r="L56" s="12" t="str">
         <f t="shared" si="103"/>
         <v/>
       </c>
-      <c r="M56" s="18" t="str">
+      <c r="M56" s="12" t="str">
         <f t="shared" si="104"/>
         <v/>
       </c>
-      <c r="N56" s="18">
+      <c r="N56" s="12">
         <f t="shared" si="105"/>
         <v>770.3199771689159</v>
       </c>
-      <c r="O56" s="18">
+      <c r="O56" s="12">
         <f t="shared" si="106"/>
         <v>868.5919142314068</v>
       </c>
-      <c r="P56" s="18">
+      <c r="P56" s="12">
         <f t="shared" si="107"/>
         <v>966.2489513569916</v>
       </c>
-      <c r="Q56" s="18">
+      <c r="Q56" s="12">
         <f t="shared" si="108"/>
         <v>1021.3105381227897</v>
       </c>
-      <c r="R56" s="18">
+      <c r="R56" s="12">
         <f t="shared" si="109"/>
         <v>1036.1476391296915</v>
       </c>
-      <c r="S56" s="18">
+      <c r="S56" s="12">
         <f t="shared" si="110"/>
         <v>1075.2170013728414</v>
       </c>
-      <c r="W56" s="12"/>
+      <c r="W56" s="17"/>
       <c r="X56" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="Y56" s="18" t="str">
+      <c r="Y56" s="12" t="str">
         <f t="shared" si="111"/>
         <v/>
       </c>
-      <c r="Z56" s="18" t="str">
+      <c r="Z56" s="12" t="str">
         <f t="shared" si="112"/>
         <v/>
       </c>
-      <c r="AA56" s="18" t="str">
+      <c r="AA56" s="12" t="str">
         <f t="shared" si="113"/>
         <v/>
       </c>
-      <c r="AB56" s="18" t="str">
+      <c r="AB56" s="12" t="str">
         <f t="shared" si="114"/>
         <v/>
       </c>
-      <c r="AC56" s="18" t="str">
+      <c r="AC56" s="12" t="str">
         <f t="shared" si="115"/>
         <v/>
       </c>
-      <c r="AD56" s="18" t="str">
+      <c r="AD56" s="12" t="str">
         <f t="shared" si="116"/>
         <v/>
       </c>
-      <c r="AE56" s="18" t="str">
+      <c r="AE56" s="12" t="str">
         <f t="shared" si="117"/>
         <v/>
       </c>
-      <c r="AF56" s="18" t="str">
+      <c r="AF56" s="12" t="str">
         <f t="shared" si="118"/>
         <v/>
       </c>
-      <c r="AG56" s="18" t="str">
+      <c r="AG56" s="12" t="str">
         <f t="shared" si="119"/>
         <v/>
       </c>
-      <c r="AH56" s="18">
+      <c r="AH56" s="12">
         <f t="shared" si="120"/>
         <v>1953.3539799756459</v>
       </c>
-      <c r="AI56" s="18">
+      <c r="AI56" s="12">
         <f t="shared" si="121"/>
         <v>1136.2146880424532</v>
       </c>
-      <c r="AJ56" s="18">
+      <c r="AJ56" s="12">
         <f t="shared" si="122"/>
         <v>459.92307948426867</v>
       </c>
-      <c r="AK56" s="18">
+      <c r="AK56" s="12">
         <f t="shared" si="123"/>
         <v>160.10081097573257</v>
       </c>
-      <c r="AL56" s="18">
+      <c r="AL56" s="12">
         <f t="shared" si="124"/>
         <v>51.46503898491946</v>
       </c>
-      <c r="AM56" s="18">
+      <c r="AM56" s="12">
         <f t="shared" si="125"/>
         <v>41.392266296184381</v>
       </c>
     </row>
     <row r="57" spans="3:39" ht="18.399999999999999" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="E57" s="19"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="19"/>
-      <c r="H57" s="19"/>
-      <c r="I57" s="19"/>
-      <c r="J57" s="19"/>
-      <c r="K57" s="19"/>
-      <c r="L57" s="19"/>
-      <c r="M57" s="19"/>
-      <c r="N57" s="19"/>
-      <c r="O57" s="19"/>
-      <c r="P57" s="19"/>
-      <c r="Q57" s="19"/>
-      <c r="R57" s="19"/>
-      <c r="S57" s="19"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="13"/>
+      <c r="K57" s="13"/>
+      <c r="L57" s="13"/>
+      <c r="M57" s="13"/>
+      <c r="N57" s="13"/>
+      <c r="O57" s="13"/>
+      <c r="P57" s="13"/>
+      <c r="Q57" s="13"/>
+      <c r="R57" s="13"/>
+      <c r="S57" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AQ26:AQ37"/>
+    <mergeCell ref="AS24:BG24"/>
     <mergeCell ref="C26:C37"/>
     <mergeCell ref="E43:S43"/>
     <mergeCell ref="C45:C56"/>
@@ -8066,8 +8068,6 @@
     <mergeCell ref="Y43:AM43"/>
     <mergeCell ref="W45:W56"/>
     <mergeCell ref="E24:S24"/>
-    <mergeCell ref="AQ26:AQ37"/>
-    <mergeCell ref="AS24:BG24"/>
   </mergeCells>
   <conditionalFormatting sqref="G34">
     <cfRule type="colorScale" priority="8">

</xml_diff>